<commit_message>
React - Learned JSX
</commit_message>
<xml_diff>
--- a/Resources/JS/JS Roadmap.xlsx
+++ b/Resources/JS/JS Roadmap.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rahul\Personal\Web Development\Resources\JS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FA67CF-2C14-46B6-822A-00EB2A4F1AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C99F07C8-2061-496E-9F70-342FE68A7FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{E53041A4-243D-437B-B283-78C7DE9CBAB2}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="243">
   <si>
     <t>#</t>
   </si>
@@ -1844,8 +1844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8B37C1D-F0D7-4E62-A284-32C7F24C94B3}">
   <dimension ref="A1:E147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="E114" sqref="E114"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="E148" sqref="E148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2698,7 +2698,9 @@
       <c r="D69" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E69" s="3"/>
+      <c r="E69" s="3" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
@@ -2830,7 +2832,9 @@
       <c r="D81" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E81" s="3"/>
+      <c r="E81" s="3" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
@@ -2841,7 +2845,9 @@
       <c r="D82" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="E82" s="3"/>
+      <c r="E82" s="3" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
@@ -2918,7 +2924,9 @@
       <c r="D89" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="E89" s="3"/>
+      <c r="E89" s="3" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
@@ -2929,7 +2937,9 @@
       <c r="D90" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="E90" s="3"/>
+      <c r="E90" s="3" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
@@ -3017,7 +3027,9 @@
       <c r="D98" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="E98" s="3"/>
+      <c r="E98" s="3" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
@@ -3061,7 +3073,9 @@
       <c r="D102" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="E102" s="3"/>
+      <c r="E102" s="3" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="3"/>
@@ -3072,7 +3086,9 @@
       <c r="D103" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="E103" s="3"/>
+      <c r="E103" s="3" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="3"/>
@@ -3083,7 +3099,9 @@
       <c r="D104" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="E104" s="3"/>
+      <c r="E104" s="3" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="3"/>
@@ -3193,7 +3211,9 @@
       <c r="D114" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="E114" s="3"/>
+      <c r="E114" s="3" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="3"/>
@@ -3259,7 +3279,9 @@
       <c r="D120" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="E120" s="3"/>
+      <c r="E120" s="3" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="3"/>
@@ -3292,7 +3314,9 @@
       <c r="D123" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="E123" s="3"/>
+      <c r="E123" s="3" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="3"/>
@@ -3303,7 +3327,9 @@
       <c r="D124" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="E124" s="3"/>
+      <c r="E124" s="3" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="3"/>
@@ -3430,7 +3456,9 @@
       <c r="D135" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="E135" s="3"/>
+      <c r="E135" s="3" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="3"/>

</xml_diff>